<commit_message>
aula dia 10 11
</commit_message>
<xml_diff>
--- a/Aula3/Ex PROVC.xlsx
+++ b/Aula3/Ex PROVC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Empreendedor\Aulas Excel Basico\fenrir\Aula3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u100054\Desktop\aprendizado\Aulas Excel Basico\Fenrir\Aula3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1662,13 +1662,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="24" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="6" borderId="24" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="25" xfId="26" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="6" borderId="25" xfId="14" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="25" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="6" borderId="25" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="26" xfId="26" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="6" borderId="26" xfId="14" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="29" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="3" fillId="2" borderId="25" xfId="26" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="2" borderId="25" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1756,6 +1752,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1765,9 +1764,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1798,6 +1794,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="6" borderId="24" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="13" fillId="6" borderId="25" xfId="14" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="6" borderId="25" xfId="25" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="13" fillId="6" borderId="26" xfId="14" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="20% - Ênfase1" xfId="25" builtinId="30"/>
@@ -2254,7 +2254,7 @@
   <dimension ref="B1:C99"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2267,14 +2267,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="91" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="98"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="2:3" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
@@ -2287,52 +2287,52 @@
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="64"/>
+      <c r="C6" s="60"/>
     </row>
     <row r="7" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="64"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="64"/>
+      <c r="C8" s="60"/>
     </row>
     <row r="9" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="64"/>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="64"/>
+      <c r="C10" s="60"/>
     </row>
     <row r="11" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="60"/>
     </row>
     <row r="12" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="60"/>
     </row>
     <row r="13" spans="2:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:3" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -2577,7 +2577,7 @@
   <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3553,7 +3553,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3572,7 +3572,7 @@
     <row r="1" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A1"/>
       <c r="B1"/>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="67" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3598,7 +3598,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="32"/>
-      <c r="C5" s="86"/>
+      <c r="C5" s="82"/>
     </row>
     <row r="6" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
@@ -3610,7 +3610,7 @@
         <v>83</v>
       </c>
       <c r="B7" s="32"/>
-      <c r="C7" s="86"/>
+      <c r="C7" s="82"/>
     </row>
     <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
@@ -3622,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="32"/>
-      <c r="C9" s="85"/>
+      <c r="C9" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
@@ -3639,7 +3639,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3661,7 +3661,7 @@
       <c r="C1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="89" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       <c r="C2" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="94">
+      <c r="D2" s="90">
         <v>5.5</v>
       </c>
     </row>
@@ -3689,7 +3689,7 @@
       <c r="C3" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="94">
+      <c r="D3" s="90">
         <v>12.2</v>
       </c>
     </row>
@@ -3703,7 +3703,7 @@
       <c r="C4" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="94">
+      <c r="D4" s="90">
         <v>12</v>
       </c>
     </row>
@@ -3717,7 +3717,7 @@
       <c r="C5" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="94">
+      <c r="D5" s="90">
         <v>28</v>
       </c>
     </row>
@@ -3731,7 +3731,7 @@
       <c r="C6" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="94">
+      <c r="D6" s="90">
         <v>41</v>
       </c>
     </row>
@@ -3745,7 +3745,7 @@
       <c r="C7" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="94">
+      <c r="D7" s="90">
         <v>35.5</v>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       <c r="C8" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="94">
+      <c r="D8" s="90">
         <v>22</v>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       <c r="C9" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="90">
         <v>35</v>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
       <c r="C10" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="94">
+      <c r="D10" s="90">
         <v>35</v>
       </c>
     </row>
@@ -3801,7 +3801,7 @@
       <c r="C11" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="94">
+      <c r="D11" s="90">
         <v>20</v>
       </c>
     </row>
@@ -3815,7 +3815,7 @@
       <c r="C12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="94">
+      <c r="D12" s="90">
         <v>18.899999999999999</v>
       </c>
     </row>
@@ -3829,7 +3829,7 @@
       <c r="C13" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="94">
+      <c r="D13" s="90">
         <v>21</v>
       </c>
     </row>
@@ -3843,7 +3843,7 @@
       <c r="C14" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="94">
+      <c r="D14" s="90">
         <v>60</v>
       </c>
     </row>
@@ -3857,7 +3857,7 @@
       <c r="C15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="94">
+      <c r="D15" s="90">
         <v>61</v>
       </c>
     </row>
@@ -3871,7 +3871,7 @@
       <c r="C16" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="94">
+      <c r="D16" s="90">
         <v>12</v>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       <c r="C17" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="94">
+      <c r="D17" s="90">
         <v>39.99</v>
       </c>
     </row>
@@ -3902,7 +3902,7 @@
   <dimension ref="A2:J23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3931,29 +3931,29 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="E5" s="95" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="E5" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="97"/>
+      <c r="B6" s="94"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="80" t="s">
         <v>116</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -3976,176 +3976,176 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="82">
+      <c r="A8" s="78">
         <v>0</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="78">
         <v>99</v>
       </c>
-      <c r="C8" s="69">
+      <c r="C8" s="65">
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="78">
         <v>40</v>
       </c>
-      <c r="G8" s="83">
+      <c r="G8" s="79">
         <v>3200</v>
       </c>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="82">
+      <c r="A9" s="78">
         <v>100</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="78">
         <v>299</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="65">
         <v>0.03</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="78">
         <v>250</v>
       </c>
-      <c r="G9" s="83">
+      <c r="G9" s="79">
         <v>20000</v>
       </c>
-      <c r="H9" s="80"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="66"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="82">
+      <c r="A10" s="78">
         <v>300</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="78">
         <v>499</v>
       </c>
-      <c r="C10" s="69">
+      <c r="C10" s="65">
         <v>0.04</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="82">
+      <c r="F10" s="78">
         <v>500</v>
       </c>
-      <c r="G10" s="83">
+      <c r="G10" s="79">
         <v>40000</v>
       </c>
-      <c r="H10" s="80"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="67"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="63"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82">
+      <c r="A11" s="78">
         <v>500</v>
       </c>
-      <c r="B11" s="82">
+      <c r="B11" s="78">
         <v>799</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="65">
         <v>0.05</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="82">
+      <c r="F11" s="78">
         <v>750</v>
       </c>
-      <c r="G11" s="83">
+      <c r="G11" s="79">
         <v>60000</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="66"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="82">
+      <c r="A12" s="78">
         <v>800</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="78">
         <v>999</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="65">
         <v>0.06</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="78">
         <v>900</v>
       </c>
-      <c r="G12" s="83">
+      <c r="G12" s="79">
         <v>72000</v>
       </c>
-      <c r="H12" s="80"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="66"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82">
+      <c r="A13" s="78">
         <v>1000</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="78">
         <v>1499</v>
       </c>
-      <c r="C13" s="69">
+      <c r="C13" s="65">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="82">
+      <c r="F13" s="78">
         <v>1200</v>
       </c>
-      <c r="G13" s="83">
+      <c r="G13" s="79">
         <v>96000</v>
       </c>
-      <c r="H13" s="80"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="66"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="82">
+      <c r="A14" s="78">
         <v>1500</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="69">
+      <c r="C14" s="65">
         <v>0.1</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="82">
+      <c r="F14" s="78">
         <v>2000</v>
       </c>
-      <c r="G14" s="83">
+      <c r="G14" s="79">
         <v>160000</v>
       </c>
-      <c r="H14" s="80"/>
-      <c r="I14" s="81"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="82">
+      <c r="F15" s="78">
         <v>3500</v>
       </c>
-      <c r="G15" s="83">
+      <c r="G15" s="79">
         <v>280000</v>
       </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16"/>
@@ -4190,7 +4190,7 @@
   <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4205,154 +4205,154 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="103" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="92">
+      <c r="B5" s="88">
         <v>0.18</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="101"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="97"/>
     </row>
     <row r="7" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="104"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F8" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="50">
         <v>9000</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="50">
         <v>3200</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="79"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="75"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="51">
         <v>1900</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="79"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="56">
+      <c r="B12" s="52">
         <v>4500</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="79"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="75"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="42"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="106"/>
+      <c r="B17" s="102"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
@@ -4366,7 +4366,7 @@
       <c r="A19" s="45">
         <v>1500</v>
       </c>
-      <c r="B19" s="46">
+      <c r="B19" s="105">
         <v>0</v>
       </c>
       <c r="D19" s="1"/>
@@ -4374,10 +4374,10 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="47">
+      <c r="A20" s="46">
         <v>2500</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B20" s="106">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D20" s="1"/>
@@ -4385,18 +4385,18 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="49">
+      <c r="A21" s="47">
         <v>4000</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="107">
         <v>0.08</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51">
+      <c r="A22" s="48">
         <v>7000</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="108">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>